<commit_message>
smol refactoring code for generate_report
</commit_message>
<xml_diff>
--- a/downloads/telestat_team.xlsx
+++ b/downloads/telestat_team.xlsx
@@ -19,6 +19,8 @@
     <sheet name="report_2024_05_21-062618" sheetId="14" state="visible" r:id="rId14"/>
     <sheet name="report_2024_05_21-215024" sheetId="15" state="visible" r:id="rId15"/>
     <sheet name="report_2024_05_21-215304" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="report_2024_05_23-180202" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="report_2024_05_23-180444" sheetId="18" state="visible" r:id="rId18"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -3676,6 +3678,840 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Активность</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Среднее количество</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Среднее количество просмотров</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>Среднее количество реакций</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>Среднее количество репостов</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>Username</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>Имя</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>Язык пользователя</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>Дата подписки на канал</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="inlineStr">
+        <is>
+          <t>Статус подписчика</t>
+        </is>
+      </c>
+      <c r="G6" s="2" t="inlineStr">
+        <is>
+          <t>Это бот?</t>
+        </is>
+      </c>
+      <c r="H6" s="2" t="inlineStr">
+        <is>
+          <t>Фото</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>6334939722</v>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>Kotellobot</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>Kotello</t>
+        </is>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>45428.03388888889</v>
+      </c>
+      <c r="F7" s="2" t="inlineStr">
+        <is>
+          <t>ADMINISTRATOR</t>
+        </is>
+      </c>
+      <c r="G7" s="2" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="H7" s="2" t="inlineStr">
+        <is>
+          <t>AQADAgADNcoxG3l1YUkAEAMAA0qCl3kBAANJcV2E92MitwAEHgQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>7182313761</v>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>mpolsh</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>Mikhail</t>
+        </is>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>45426.68694444445</v>
+      </c>
+      <c r="F8" s="2" t="inlineStr">
+        <is>
+          <t>ADMINISTRATOR</t>
+        </is>
+      </c>
+      <c r="G8" s="2" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="H8" s="2" t="inlineStr">
+        <is>
+          <t>Фото отсутствует</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>6001084404</v>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>MPolsh_practicum_bot</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>Практикум статус</t>
+        </is>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>45424.02155092593</v>
+      </c>
+      <c r="F9" s="2" t="inlineStr">
+        <is>
+          <t>ADMINISTRATOR</t>
+        </is>
+      </c>
+      <c r="G9" s="2" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="H9" s="2" t="inlineStr">
+        <is>
+          <t>AQADAgADJ84xGw7fKUsAEAMAA_RHsWUBAAMZ__beDZvlZwAEHgQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>6361686464</v>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>KrivolapDmitriyBot</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>People</t>
+        </is>
+      </c>
+      <c r="E10" s="3" t="n">
+        <v>45413.04180555556</v>
+      </c>
+      <c r="F10" s="2" t="inlineStr">
+        <is>
+          <t>ADMINISTRATOR</t>
+        </is>
+      </c>
+      <c r="G10" s="2" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="H10" s="2" t="inlineStr">
+        <is>
+          <t>AQADAgADZtExG2EWuEoAEAMAA8ChL3sBAAPo15zKYGsragAEHgQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>1692872509</v>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>Kastet1991</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>Константин</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>ru</t>
+        </is>
+      </c>
+      <c r="E11" s="3" t="n">
+        <v>45408.84982638889</v>
+      </c>
+      <c r="F11" s="2" t="inlineStr">
+        <is>
+          <t>MEMBER</t>
+        </is>
+      </c>
+      <c r="G11" s="2" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="H11" s="2" t="inlineStr">
+        <is>
+          <t>AQADAgADvMoxG5dH0EgAEAMAAz0v52QABH8iLqYgORzcAAQeBA</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>865687262</v>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>orbikadm</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="E12" s="3" t="n">
+        <v>45408.57420138889</v>
+      </c>
+      <c r="F12" s="2" t="inlineStr">
+        <is>
+          <t>MEMBER</t>
+        </is>
+      </c>
+      <c r="G12" s="2" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="H12" s="2" t="inlineStr">
+        <is>
+          <t>AQADAgADqacxG95WmTMAEAMAA95WmTMABKTUh0ReeboiAAQeBA</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>1678917129</v>
+      </c>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>dk06789</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="inlineStr">
+        <is>
+          <t>Dmitry</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="E13" s="3" t="n">
+        <v>45408.53905092592</v>
+      </c>
+      <c r="F13" s="2" t="inlineStr">
+        <is>
+          <t>MEMBER</t>
+        </is>
+      </c>
+      <c r="G13" s="2" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="H13" s="2" t="inlineStr">
+        <is>
+          <t>AQADAgADcbIxG3-xIUoAEAMAAwk-EmQABCEK7Z_QlQtCAAQeBA</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n">
+        <v>6270434089</v>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>MaksInsceBot</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="inlineStr">
+        <is>
+          <t>ТестБот</t>
+        </is>
+      </c>
+      <c r="E14" s="3" t="n">
+        <v>45408.53241898148</v>
+      </c>
+      <c r="F14" s="2" t="inlineStr">
+        <is>
+          <t>ADMINISTRATOR</t>
+        </is>
+      </c>
+      <c r="G14" s="2" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="H14" s="2" t="inlineStr">
+        <is>
+          <t>Фото отсутствует</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n">
+        <v>51297554</v>
+      </c>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>Maks_insurance</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="inlineStr">
+        <is>
+          <t>Максим</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>ru</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>Отсутствует для владельца</t>
+        </is>
+      </c>
+      <c r="F15" s="2" t="inlineStr">
+        <is>
+          <t>OWNER</t>
+        </is>
+      </c>
+      <c r="G15" s="2" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="H15" s="2" t="inlineStr">
+        <is>
+          <t>Фото отсутствует</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Активность</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Среднее количество</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Среднее количество просмотров</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>Среднее количество реакций</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>Среднее количество репостов</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>Username</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>Имя</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>Язык пользователя</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>Дата подписки на канал</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="inlineStr">
+        <is>
+          <t>Статус подписчика</t>
+        </is>
+      </c>
+      <c r="G6" s="2" t="inlineStr">
+        <is>
+          <t>Это бот?</t>
+        </is>
+      </c>
+      <c r="H6" s="2" t="inlineStr">
+        <is>
+          <t>Фото</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>6334939722</v>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>Kotellobot</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>Kotello</t>
+        </is>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>45428.03388888889</v>
+      </c>
+      <c r="F7" s="2" t="inlineStr">
+        <is>
+          <t>ADMINISTRATOR</t>
+        </is>
+      </c>
+      <c r="G7" s="2" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="H7" s="2" t="inlineStr">
+        <is>
+          <t>AQADAgADNcoxG3l1YUkAEAMAA0qCl3kBAANJcV2E92MitwAEHgQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>7182313761</v>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>mpolsh</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>Mikhail</t>
+        </is>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>45426.68694444445</v>
+      </c>
+      <c r="F8" s="2" t="inlineStr">
+        <is>
+          <t>ADMINISTRATOR</t>
+        </is>
+      </c>
+      <c r="G8" s="2" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="H8" s="2" t="inlineStr">
+        <is>
+          <t>Фото отсутствует</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>6001084404</v>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>MPolsh_practicum_bot</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>Практикум статус</t>
+        </is>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>45424.02155092593</v>
+      </c>
+      <c r="F9" s="2" t="inlineStr">
+        <is>
+          <t>ADMINISTRATOR</t>
+        </is>
+      </c>
+      <c r="G9" s="2" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="H9" s="2" t="inlineStr">
+        <is>
+          <t>AQADAgADJ84xGw7fKUsAEAMAA_RHsWUBAAMZ__beDZvlZwAEHgQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>6361686464</v>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>KrivolapDmitriyBot</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>People</t>
+        </is>
+      </c>
+      <c r="E10" s="3" t="n">
+        <v>45413.04180555556</v>
+      </c>
+      <c r="F10" s="2" t="inlineStr">
+        <is>
+          <t>ADMINISTRATOR</t>
+        </is>
+      </c>
+      <c r="G10" s="2" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="H10" s="2" t="inlineStr">
+        <is>
+          <t>AQADAgADZtExG2EWuEoAEAMAA8ChL3sBAAPo15zKYGsragAEHgQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>1692872509</v>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>Kastet1991</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>Константин</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>ru</t>
+        </is>
+      </c>
+      <c r="E11" s="3" t="n">
+        <v>45408.84982638889</v>
+      </c>
+      <c r="F11" s="2" t="inlineStr">
+        <is>
+          <t>MEMBER</t>
+        </is>
+      </c>
+      <c r="G11" s="2" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="H11" s="2" t="inlineStr">
+        <is>
+          <t>AQADAgADvMoxG5dH0EgAEAMAAz0v52QABH8iLqYgORzcAAQeBA</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>865687262</v>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>orbikadm</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="E12" s="3" t="n">
+        <v>45408.57420138889</v>
+      </c>
+      <c r="F12" s="2" t="inlineStr">
+        <is>
+          <t>MEMBER</t>
+        </is>
+      </c>
+      <c r="G12" s="2" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="H12" s="2" t="inlineStr">
+        <is>
+          <t>AQADAgADqacxG95WmTMAEAMAA95WmTMABKTUh0ReeboiAAQeBA</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>1678917129</v>
+      </c>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>dk06789</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="inlineStr">
+        <is>
+          <t>Dmitry</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>ru</t>
+        </is>
+      </c>
+      <c r="E13" s="3" t="n">
+        <v>45408.53905092592</v>
+      </c>
+      <c r="F13" s="2" t="inlineStr">
+        <is>
+          <t>MEMBER</t>
+        </is>
+      </c>
+      <c r="G13" s="2" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="H13" s="2" t="inlineStr">
+        <is>
+          <t>AQADAgADcbIxG3-xIUoAEAMAAwk-EmQABCEK7Z_QlQtCAAQeBA</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n">
+        <v>6270434089</v>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>MaksInsceBot</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="inlineStr">
+        <is>
+          <t>ТестБот</t>
+        </is>
+      </c>
+      <c r="E14" s="3" t="n">
+        <v>45408.53241898148</v>
+      </c>
+      <c r="F14" s="2" t="inlineStr">
+        <is>
+          <t>ADMINISTRATOR</t>
+        </is>
+      </c>
+      <c r="G14" s="2" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="H14" s="2" t="inlineStr">
+        <is>
+          <t>Фото отсутствует</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n">
+        <v>51297554</v>
+      </c>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>Maks_insurance</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="inlineStr">
+        <is>
+          <t>Максим</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>ru</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>Отсутствует для владельца</t>
+        </is>
+      </c>
+      <c r="F15" s="2" t="inlineStr">
+        <is>
+          <t>OWNER</t>
+        </is>
+      </c>
+      <c r="G15" s="2" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="H15" s="2" t="inlineStr">
+        <is>
+          <t>Фото отсутствует</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>